<commit_message>
Array size is now 7800
</commit_message>
<xml_diff>
--- a/AverageTimes.xlsx
+++ b/AverageTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brittany\SortingAlgorithmJava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC1CEF22-6404-466A-9E3D-105A0B8CC6AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2C013D-7B1A-498D-8280-C6D18F5FFFC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F33F5116-A191-4DA9-8EED-3A2C07EBA289}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Selection Sort</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>C++</t>
   </si>
 </sst>
 </file>
@@ -235,6 +244,102 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B2AA-4DD3-9FE9-C73714F92AF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3028-4E72-A0F3-CACB684B9427}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3028-4E72-A0F3-CACB684B9427}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1293,21 +1398,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A591C-B3D2-4516-9A89-F060B6582EE3}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5.5</v>
       </c>
@@ -1333,6 +1439,60 @@
       </c>
       <c r="D2">
         <v>11.9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>5.5</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>14.7</v>
+      </c>
+      <c r="E22">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created graphs for averages
</commit_message>
<xml_diff>
--- a/AverageTimes.xlsx
+++ b/AverageTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brittany\SortingAlgorithmJava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2C013D-7B1A-498D-8280-C6D18F5FFFC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484BB504-2726-4B83-AB76-431E80D8836F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F33F5116-A191-4DA9-8EED-3A2C07EBA289}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Selection Sort</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>C++</t>
+  </si>
+  <si>
+    <t>Average for arrays size of 7800</t>
+  </si>
+  <si>
+    <t>Array of size 1000</t>
   </si>
 </sst>
 </file>
@@ -286,6 +292,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -515,7 +524,1859 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>C++ Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Times for array size 7800</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:ofPieChart>
+        <c:ofPieType val="pie"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-1EC5-44C6-B715-8D8E40B7283B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1EC5-44C6-B715-8D8E40B7283B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1EC5-44C6-B715-8D8E40B7283B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-1EC5-44C6-B715-8D8E40B7283B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2095144356955383E-2"/>
+                  <c:y val="-0.1921289005540974"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4D06ED60-14E1-4198-8897-F8CF11DD0465}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1EC5-44C6-B715-8D8E40B7283B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.1748250218722661E-2"/>
+                  <c:y val="0.20220217264508603"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B55A91CF-4E2F-409E-9484-F6B0902E3AD7}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1EC5-44C6-B715-8D8E40B7283B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.19810837707786527"/>
+                  <c:y val="-5.3206838728492273E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6962CABE-DEDD-465E-ADE3-322F8AE3C174}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1EC5-44C6-B715-8D8E40B7283B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B514CFEE-E078-4D26-8B19-BD7EDA03106B}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-1EC5-44C6-B715-8D8E40B7283B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$E$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>188.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>229.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1EC5-44C6-B715-8D8E40B7283B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:secondPieSize val="75"/>
+        <c:serLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:serLines>
+      </c:ofPieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Python </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1440" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Times for array size 7800</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:ofPieChart>
+        <c:ofPieType val="pie"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BB905428-21E7-4607-81F7-3311AD4F76DF}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{476B60F3-6180-4F44-B05A-292068FAB176}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.17394006999125108"/>
+                  <c:y val="-5.0815106445027708E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{08DA1F7B-7253-461C-A2EB-57610610415B}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BFE245F6-975A-4B97-B620-FB182405C74F}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$E$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5483.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11825.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>290.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE58-40CE-BED1-F7A5B38D2EE7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:secondPieSize val="75"/>
+        <c:serLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:serLines>
+      </c:ofPieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Java </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Times for array size 7800</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.14356146106736659"/>
+                  <c:y val="-2.2822251385243512E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2FCB1FB6-0163-49F4-BB16-8BCBA69096BD}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6D5FC609-54C3-4C97-A3EC-D6A93B879E28}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.2453083989501311E-2"/>
+                  <c:y val="-3.9403251676873724E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{ED0EE4B8-C933-446B-B2C7-4E72D5B7EECB}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:sysClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9558180227471574E-3"/>
+                  <c:y val="1.0893117526975795E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>36.6</a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Milliseconds</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$E$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>77.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4AEA-42E1-B1B5-5D96FC5B55BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1060,20 +2921,1591 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="333">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="333">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1093,6 +4525,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{982E8550-A0D8-4915-84ED-0DD794F1F1AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B17015B-415C-4252-9F8C-505273BD2325}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>384175</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8CFAEA0-736D-42E3-AC2C-511E78B1A1C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1400,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A591C-B3D2-4516-9A89-F060B6582EE3}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1445,13 +4985,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E4" t="s">
-        <v>6</v>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1473,30 +5013,55 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>5.5</v>
+        <v>77.2</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D22">
-        <v>14.7</v>
+        <v>23.6</v>
       </c>
       <c r="E22">
-        <v>11.9</v>
+        <v>36.6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
+      <c r="B23">
+        <v>5483.7</v>
+      </c>
+      <c r="C23">
+        <v>11825.2</v>
+      </c>
+      <c r="D23">
+        <v>290.7</v>
+      </c>
+      <c r="E23">
+        <v>59.2</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>6</v>
       </c>
+      <c r="B24">
+        <v>188.9</v>
+      </c>
+      <c r="C24">
+        <v>229.6</v>
+      </c>
+      <c r="D24">
+        <v>1.2</v>
+      </c>
+      <c r="E24">
+        <v>0.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed wrong number for the number of lines of code for QS
</commit_message>
<xml_diff>
--- a/AverageTimes.xlsx
+++ b/AverageTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brittany\SortingAlgorithmJava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484BB504-2726-4B83-AB76-431E80D8836F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6417F6E-4408-495E-AD9F-7E26AE9B99BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F33F5116-A191-4DA9-8EED-3A2C07EBA289}"/>
   </bookViews>
@@ -712,6 +712,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-AEA5-45A0-A41F-57F19202B484}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -4940,8 +4945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A591C-B3D2-4516-9A89-F060B6582EE3}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>